<commit_message>
Updated use cases so that students no longer have to login.
</commit_message>
<xml_diff>
--- a/use cases.xlsx
+++ b/use cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="71">
   <si>
     <t>Nr. Pas</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Se introduc credențialele adminului și se apasă login.</t>
   </si>
   <si>
-    <t>Adminul este întâmpinat de pagina de unde se pot vizualiza utilizatorii curenți ai aplicației (profesori și studenți).</t>
-  </si>
-  <si>
     <t>Se apasă click pe butonul "Adăugare".</t>
   </si>
   <si>
@@ -226,6 +223,12 @@
   </si>
   <si>
     <t>Va apărea pe ecran un formular unde se poate introduce parola curentă, parola dorită si confirmarea parolei dorite.</t>
+  </si>
+  <si>
+    <t>Se apasă link-ul "Continuă ca student".</t>
+  </si>
+  <si>
+    <t>Adminul este întâmpinat de pagina de unde se pot vizualiza utilizatorii curenți ai aplicației (profesori).</t>
   </si>
 </sst>
 </file>
@@ -651,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -758,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>7</v>
@@ -806,7 +809,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
@@ -838,10 +841,10 @@
         <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="45">
@@ -849,10 +852,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30">
@@ -860,7 +863,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>7</v>
@@ -882,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1051,7 +1054,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
@@ -1121,7 +1124,7 @@
         <v>47</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30">
@@ -1212,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>46</v>
@@ -1255,7 +1258,7 @@
         <v>49</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="45">
@@ -1263,10 +1266,10 @@
         <v>3</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="45">
@@ -1274,7 +1277,7 @@
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>7</v>
@@ -1285,15 +1288,15 @@
         <v>5</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="10"/>
@@ -1328,7 +1331,7 @@
         <v>49</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="45">
@@ -1336,10 +1339,10 @@
         <v>3</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1355,13 +1358,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1372,7 +1375,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1416,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>40</v>

</xml_diff>